<commit_message>
add experiments for gpa and curran
</commit_message>
<xml_diff>
--- a/output/funa/date01022024/output.xlsx
+++ b/output/funa/date01022024/output.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuenl-my.sharepoint.com/personal/r_m_schouten_tue_nl/Documents/Documents/Github/DescriptionModels/output/funa/date01022024/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_CB0AA26A6800F24653FEC50771184473BE404447" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-47040" yWindow="960" windowWidth="14400" windowHeight="10665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation_summary" sheetId="1" r:id="rId1"/>
     <sheet name="analysis_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>data_key</t>
   </si>
@@ -191,9 +197,6 @@
     <t>desc</t>
   </si>
   <si>
-    <t>zsubrange_low</t>
-  </si>
-  <si>
     <t>subrange_fit</t>
   </si>
   <si>
@@ -203,22 +206,13 @@
     <t>{'n_consd': 184, 'n_sim_descs': 24, 'n_small_groups': 14, 'n_redun_decs': None}</t>
   </si>
   <si>
-    <t>{'n_consd': 3651, 'n_sim_descs': 547, 'n_small_groups': 356, 'n_redun_decs': 13}</t>
-  </si>
-  <si>
-    <t>{'n_consd': 3626, 'n_sim_descs': 554, 'n_small_groups': 818, 'n_redun_decs': 1}</t>
-  </si>
-  <si>
-    <t>{'n_consd': 3646, 'n_sim_descs': 528, 'n_small_groups': 415, 'n_redun_decs': 13, 'n_redun_descs': 2}</t>
-  </si>
-  <si>
-    <t>{'n_consd': 3667, 'n_sim_descs': 203, 'n_small_groups': 2920, 'n_redun_decs': 0, 'n_redun_descs': 0}</t>
-  </si>
-  <si>
-    <t>{'n_consd': 12, 'n_small_groups': 0, 'n_redun_decs': 1}</t>
-  </si>
-  <si>
-    <t>{'n_consd': 18, 'n_small_groups': 0, 'n_redun_decs': 0}</t>
+    <t>{'n_consd': 3653, 'n_sim_descs': 577, 'n_small_groups': 468, 'n_redun_decs': 1}</t>
+  </si>
+  <si>
+    <t>{'n_consd': 3675, 'n_sim_descs': 468, 'n_small_groups': 1269, 'n_redun_decs': 4, 'n_redun_descs': 0}</t>
+  </si>
+  <si>
+    <t>{'n_consd': 10, 'n_small_groups': 0, 'n_redun_decs': 0}</t>
   </si>
   <si>
     <t>['f3fa-babe66', 'f3fa-bafe19', 'f3fa-bafe55', 'f3fa-bafo84', 'f3fa-bafy34', 'f3fa-bajo437', 'f3fa-bako357', 'f3fa-baku638', 'f3fa-balu481', 'f3fa-bamu72', 'f3fa-bane815', 'f3fa-bany90', 'f3fa-baqy06', 'f3fa-baqy64', 'f3fa-base67', 'f3fa-base95', 'f3fa-bato80', 'f3fa-bavo53', 'f3fa-bavu67', 'f3fa-bebe398', 'f3fa-bebu43', 'f3fa-beco412', 'f3fa-beje81', 'f3fa-bejy62', 'f3fa-beka576', 'f3fa-beky153', 'f3fa-bela30', 'f3fa-belo97', 'f3fa-bemo09', 'f3fa-bepe30', 'f3fa-bepo46', 'f3fa-bera26', 'f3fa-bera838', 'f3fa-bere54', 'f3fa-bero18', 'f3fa-bese02', 'f3fa-beti83', 'f3fa-bevy51', 'f3fa-bexe44', 'f3fa-bexi300', 'f3fa-bezi96', 'f3fa-bezo90', 'f3fa-bezu74', 'f3fa-bezu87', 'f3fa-biba792', 'f3fa-bici69', 'f3fa-bicu32', 'f3fa-bige13', 'f3fa-bige58', 'f3fa-bigo365', 'f3fa-bigu44', 'f3fa-bigu72', 'f3fa-bigy34', 'f3fa-bijo68', 'f3fa-bike448', 'f3fa-biky34', 'f3fa-bile093', 'f3fa-bilu35', 'f3fa-bimo68', 'f3fa-bire856', 'f3fa-bito53', 'f3fa-bity31', 'f3fa-bixa66', 'f3fa-bixe65', 'f3fa-bizi40', 'f3fa-bobo27', 'f3fa-boca190', 'f3fa-boco628', 'f3fa-boco71', 'f3fa-bodo15', 'f3fa-bofa59', 'f3fa-bofo60', 'f3fa-bogi29', 'f3fa-boje11', 'f3fa-boje82', 'f3fa-boky29', 'f3fa-bolu326', 'f3fa-bony68', 'f3fa-boso20', 'f3fa-bota35', 'f3fa-bovu39', 'f3fa-boxe04', 'f3fa-bozo184', 'f3fa-bozu00', 'f3fa-bubu357', 'f3fa-bucy95', 'f3fa-bufe37', 'f3fa-bufi510', 'f3fa-bufu89', 'f3fa-bufy35', 'f3fa-bugi90', 'f3fa-bugu25', 'f3fa-buja24', 'f3fa-buje54', 'f3fa-bujy226', 'f3fa-bumi29', 'f3fa-buni312', 'f3fa-buxi831', 'f3fa-buxo68', 'f3fa-buxy67', 'f3fa-buzi87', 'f3fa-byby673', 'f3fa-byca03', 'f3fa-byco456', 'f3fa-byco473', 'f3fa-bydu714', 'f3fa-bydu95', 'f3fa-byfu83', 'f3fa-byga00', 'f3fa-byga60', 'f3fa-byge609', 'f3fa-bygi56', 'f3fa-byhu539', 'f3fa-byka10', 'f3fa-bylo71', 'f3fa-bylu424', 'f3fa-byma976', 'f3fa-bymy706', 'f3fa-bynu41', 'f3fa-bynu93', 'f3fa-bypa422', 'f3fa-byty42', 'f3fa-byvi09', 'f3fa-byxy85', 'f3fa-byza182', 'f3fa-byzi73', 'f3fa-caba91', 'f3fa-cabo55', 'f3fa-caby644', 'f3fa-caca71', 'f3fa-caca85', 'f3fa-cacy69', 'f3fa-cade38', 'f3fa-cady63', 'f3fa-cafa873', 'f3fa-cafe661', 'f3fa-cafo75', 'f3fa-caga84', 'f3fa-cage22', 'f3fa-cagu23', 'f3fa-caje475', 'f3fa-cajo23', 'f3fa-camy56', 'f3fa-cana216', 'f3fa-caqi59', 'f3fa-caqy30', 'f3fa-cary61', 'f3fa-case059', 'f3fa-casu01', 'f3fa-cate58', 'f3fa-cati12', 'f3fa-caty09', 'f3fa-cavi94', 'f3fa-caza237', 'f3fa-cazi96', 'f3fa-cazo19', 'f3fa-cazy874', 'f3fa-cecy77', 'f3fa-ceke377', 'f3fa-cele07', 'f3fa-cely96', 'f3fa-cema77', 'f3fa-cepy00', 'f3fa-ceqi66', 'f3fa-cequ51', 'f3fa-cere65', 'f3fa-cere931', 'f3fa-cero10', 'f3fa-ceti70', 'f3fa-ceto113', 'f3fa-ceto283', 'f3fa-cevu90', 'f3fa-cexa35', 'f3fa-cexo97', 'f3fa-cexy725', 'f3fa-cezi44', 'f3fa-cibe88', 'f3fa-cibu013', 'f3fa-cici40', 'f3fa-cici44', 'f3fa-cidi98', 'f3fa-cidy21', 'f3fa-cige90', 'f3fa-cigo47', 'f3fa-cija378', 'f3fa-cilo583', 'f3fa-cimu15', 'f3fa-cine83', 'f3fa-ciqo248', 'f3fa-cisy041', 'f3fa-cixe114', 'f3fa-cixe35', 'f3fa-cixe568', 'f3fa-cixo949', 'f3fa-cixy80', 'f3fa-code82', 'f3fa-codi62', 'f3fa-cofi190', 'f3fa-cofy572', 'f3fa-cogi12', 'f3fa-cogu30', 'f3fa-cogu39', 'f3fa-coju92', 'f3fa-coju95', 'f3fa-coko573', 'f3fa-colu982', 'f3fa-cone242', 'f3fa-coni312', 'f3fa-copy15', 'f3fa-cose00', 'f3fa-cosi677', 'f3fa-cota87', 'f3fa-coty08', 'f3fa-coxe72', 'f3fa-coxo711', 'f3fa-cubo35', 'f3fa-cuby284', 'f3fa-cuca63', 'f3fa-cucy644', 'f3fa-cude51', 'f3fa-cudi30', 'f3fa-cuhu295', 'f3fa-cujo14', 'f3fa-cuke34', 'f3fa-cuki429', 'f3fa-culi38', 'f3fa-culi49', 'f3fa-culu037', 'f3fa-culu533', 'f3fa-cuni92', 'f3fa-cuny378', 'f3fa-cuny464', 'f3fa-cuny47', 'f3fa-cupa39', 'f3fa-cupa52', 'f3fa-cupy60', 'f3fa-cuqi15', 'f3fa-curo65', 'f3fa-cusy18', 'f3fa-cusy74', 'f3fa-cutu75', 'f3fa-cuxa87', 'f3fa-cuza07', 'f3fa-cydy531', 'f3fa-cygi368', 'f3fa-cygo67', 'f3fa-cyha327', 'f3fa-cyhe33', 'f3fa-cyhi169', 'f3fa-cyja960', 'f3fa-cyje70', 'f3fa-cyko444', 'f3fa-cyla98', 'f3fa-cylo84', 'f3fa-cylu36', 'f3fa-cyma519', 'f3fa-cymy773', 'f3fa-cyqa18', 'f3fa-cyxu938', 'f3fa-daba10', 'f3fa-daba97', 'f3fa-dabe18', 'f3fa-daby721', 'f3fa-dace300', 'f3fa-dado06', 'f3fa-dafy41', 'f3fa-dage63', 'f3fa-dagy64', 'f3fa-dahu770', 'f3fa-dake269', 'f3fa-dake83', 'f3fa-dali50', 'f3fa-dalu56', 'f3fa-damo92', 'f3fa-dana673', 'f3fa-dapa00', 'f3fa-dape63', 'f3fa-daqu58', 'f3fa-daru15', 'f3fa-dase74', 'f3fa-dasi44', 'f3fa-dasi65', 'f3fa-dasi883', 'f3fa-daso04', 'f3fa-dasu91', 'f3fa-dato616', 'f3fa-datu78', 'f3fa-daxa01', 'f3fa-daza683', 'f3fa-dece87', 'f3fa-deco028', 'f3fa-decu95', 'f3fa-dedi35', 'f3fa-dedu951', 'f3fa-degi57', 'f3fa-degu23', 'f3fa-degy84', 'f3fa-deho370', 'f3fa-dehu557', 'f3fa-deki571', 'f3fa-dema13', 'f3fa-demi213', 'f3fa-dena902', 'f3fa-depi76', 'f3fa-depy34', 'f3fa-deru56', 'f3fa-dery71', 'f3fa-dese86', 'f3fa-deve110', 'f3fa-dexu23', 'f3fa-dezi92', 'f3fa-dici44', 'f3fa-dico21', 'f3fa-dide703', 'f3fa-didi354', 'f3fa-digo669', 'f3fa-digy26', 'f3fa-dihy88', 'f3fa-dija85', 'f3fa-diju98', 'f3fa-dika40', 'f3fa-dimi75', 'f3fa-dine21', 'f3fa-diqy83', 'f3fa-dita60', 'f3fa-dita76', 'f3fa-dite92', 'f3fa-ditu67', 'f3fa-dixa72', 'f3fa-dize58', 'f3fa-dobu66', 'f3fa-doca718', 'f3fa-docu32', 'f3fa-dode40', 'f3fa-dody233', 'f3fa-dofa121', 'f3fa-dogi41', 'f3fa-dogu82', 'f3fa-dohu64', 'f3fa-doka08', 'f3fa-doke31', 'f3fa-doke46', 'f3fa-doky77', 'f3fa-doma12', 'f3fa-dome19', 'f3fa-domu639', 'f3fa-dopi84', 'f3fa-dopo54', 'f3fa-dopu329', 'f3fa-dopu35', 'f3fa-doqi471', 'f3fa-dose89', 'f3fa-doti12', 'f3fa-dubi06', 'f3fa-dubo518', 'f3fa-duby36', 'f3fa-ducy51', 'f3fa-dufy532', 'f3fa-dugi28', 'f3fa-duho645', 'f3fa-duja11', 'f3fa-duki47', 'f3fa-duko087', 'f3fa-dula97', 'f3fa-dunu09', 'f3fa-duxa368', 'f3fa-dybu080', 'f3fa-dyga75', 'f3fa-dygi78', 'f3fa-dyho17', 'f3fa-dyhy50', 'f3fa-dyja95', 'f3fa-dyjo99', 'f3fa-dyju19', 'f3fa-dyki72', 'f3fa-dyla63', 'f3fa-dylu88', 'f3fa-dyly938', 'f3fa-dymo18', 'f3fa-dyni03', 'f3fa-dyno08', 'f3fa-dyny49', 'f3fa-dyqe79', 'f3fa-dysa52', 'f3fa-dyso37', 'f3fa-dyso95', 'f3fa-dyta674', 'f3fa-dyxi33', 'f3fa-dyxy59', 'f3fa-dyze36', 'f3fa-fabi17', 'f3fa-face68', 'f3fa-fada10', 'f3fa-fafa43', 'f3fa-fafi710', 'f3fa-faha12', 'f3fa-fahe566', 'f3fa-fahi93', 'f3fa-fajo142', 'f3fa-fale54', 'f3fa-fali99', 'f3fa-fama249', 'f3fa-famu994', 'f3fa-faqu68', 'f3fa-fari84', 'f3fa-faxa66', 'f3fa-faza70', 'f3fa-fazi930', 'f3fa-fazu12', 'f3fa-fazy56', 'f3fa-feco87', 'f3fa-fede36', 'f3fa-fefo61', 'f3fa-fefy20', 'f3fa-feho04', 'f3fa-feho36', 'f3fa-felu27', 'f3fa-fepi055', 'f3fa-fepy422', 'f3fa-fepy60', 'f3fa-feqa06', 'f3fa-feqa11', 'f3fa-feqa56', 'f3fa-feri470', 'f3fa-fesy32', 'f3fa-feti59', 'f3fa-feto27', 'f3fa-fexa39', 'f3fa-fica036', 'f3fa-fica56', 'f3fa-fide28', 'f3fa-fidi44', 'f3fa-fifa55', 'f3fa-fify34', 'f3fa-figa33', 'f3fa-fige58', 'f3fa-fihu02', 'f3fa-fihu41', 'f3fa-fiju521', 'f3fa-fiki705', 'f3fa-filu44', 'f3fa-fime75', 'f3fa-fimi50', 'f3fa-fimu51', 'f3fa-fimy722', 'f3fa-fipa55', 'f3fa-fipi239', 'f3fa-fiqe68', 'f3fa-fira57', 'f3fa-fiso45', 'f3fa-fiva38', 'f3fa-fiva718', 'f3fa-fivi43', 'f3fa-fixa73', 'f3fa-fixu51', 'f3fa-fizu21', 'f3fa-foby38', 'f3fa-fofa75', 'f3fa-fofa94', 'f3fa-foge436', 'f3fa-foho249', 'f3fa-foho25', 'f3fa-fola281', 'f3fa-foli29', 'f3fa-fome30', 'f3fa-fome74', 'f3fa-fone208', 'f3fa-foqi877', 'f3fa-foqo08', 'f3fa-fose801', 'f3fa-foze977', 'f3fa-fube85', 'f3fa-fuby12', 'f3fa-fufe384', 'f3fa-fuge78', 'f3fa-fuho852', 'f3fa-fuhu794', 'f3fa-fuja76', 'f3fa-fujo64', 'f3fa-fujo81', 'f3fa-fuju228', 'f3fa-fujy745', 'f3fa-fuka528', 'f3fa-fulu828', 'f3fa-fuma518', 'f3fa-fune65', 'f3fa-fupe93', 'f3fa-fupo366', 'f3fa-fuqy558', 'f3fa-fusu02', 'f3fa-fuvi45', 'f3fa-fuxo19', 'f3fa-fuzo05', 'f3fa-fybu37', 'f3fa-fycy07', 'f3fa-fyfu56', 'f3fa-fyhu791', 'f3fa-fyko847', 'f3fa-fyku15', 'f3fa-fyna31', 'f3fa-fyne476', 'f3fa-fyni27', 'f3fa-fypi581', 'f3fa-fyry261', 'f3fa-fysa39', 'f3fa-fyso84', 'f3fa-fysu07', 'f3fa-fysu59', 'f3fa-fyte566', 'f3fa-gaby45', 'f3fa-gadu33', 'f3fa-gady485', 'f3fa-gahe96', 'f3fa-gahi301', 'f3fa-gaka90', 'f3fa-game99', 'f3fa-gamo73', 'f3fa-gani650', 'f3fa-gapa159', 'f3fa-gare03', 'f3fa-gaty80', 'f3fa-gaze953', 'f3fa-geba67', 'f3fa-geba90', 'f3fa-gebe95', 'f3fa-gebi802', 'f3fa-gebi85', 'f3fa-geco47', 'f3fa-gede31', 'f3fa-gedu77', 'f3fa-gefa44', 'f3fa-geha32', 'f3fa-geju822', 'f3fa-geme40', 'f3fa-gemo545', 'f3fa-gemu57', 'f3fa-gemu908', 'f3fa-geni37', 'f3fa-gepa887', 'f3fa-gepe617', 'f3fa-gepu50', 'f3fa-gete24', 'f3fa-gety77', 'f3fa-gexa80', 'f3fa-gezo27', 'f3fa-gezy33', 'f3fa-gida52', 'f3fa-gife49', 'f3fa-gigi20', 'f3fa-gihy77', 'f3fa-gilo60', 'f3fa-gimi05', 'f3fa-giqa42', 'f3fa-giqe571', 'f3fa-giqo48', 'f3fa-giri26', 'f3fa-gite31', 'f3fa-gitu10', 'f3fa-givu10', 'f3fa-gizu90', 'f3fa-goda386', 'f3fa-gody434', 'f3fa-gofi05', 'f3fa-gofy04', 'f3fa-gohu47', 'f3fa-goje64', 'f3fa-gojy56', 'f3fa-gola228', 'f3fa-gome80', 'f3fa-gory14', 'f3fa-gota06', 'f3fa-gove39', 'f3fa-govy21', 'f3fa-goxe91', 'f3fa-gozu457', 'f3fa-gubu16', 'f3fa-gubu85', 'f3fa-guci76', 'f3fa-gudu347', 'f3fa-gudu79', 'f3fa-gufi026', 'f3fa-gufy640', 'f3fa-guga530', 'f3fa-guke794', 'f3fa-gupe227', 'f3fa-gupe86', 'f3fa-gupo40', 'f3fa-guru24', 'f3fa-guso642', 'f3fa-gusu991', 'f3fa-guto27', 'f3fa-guvy22', 'f3fa-guvy29', 'f3fa-guxi516', 'f3fa-guza79', 'f3fa-guzi10', 'f3fa-guzu40', 'f3fa-guzy66', 'f3fa-gybe95', 'f3fa-gyfy517', 'f3fa-gyhe24', 'f3fa-gyja456', 'f3fa-gyje03', 'f3fa-gyjo674', 'f3fa-gyjy25', 'f3fa-gyjy66', 'f3fa-gyki06', 'f3fa-gyku54', 'f3fa-gymy80', 'f3fa-gyna942', 'f3fa-gypy704', 'f3fa-gyre129', 'f3fa-gysu273', 'f3fa-gyvu11', 'f3fa-gyvu97', 'f3fa-gyvy67', 'f3fa-gyvy83', 'f3fa-gyxi36', 'f3fa-gyzi12', 'f3fa-habe21', 'f3fa-hace09', 'f3fa-haci64', 'f3fa-haci742', 'f3fa-hacy625', 'f3fa-hado21', 'f3fa-hafa00', 'f3fa-haga50', 'f3fa-hage04', 'f3fa-hagi63', 'f3fa-hahi73', 'f3fa-hahy20', 'f3fa-hajy47', 'f3fa-haki19', 'f3fa-hame80', 'f3fa-hamo583', 'f3fa-hape119', 'f3fa-haqy41', 'f3fa-hasi07', 'f3fa-haty94', 'f3fa-haty97', 'f3fa-have252', 'f3fa-hefi08', 'f3fa-hegy30', 'f3fa-heha42', 'f3fa-hehy995', 'f3fa-hejo44', 'f3fa-heko782', 'f3fa-hemi702', 'f3fa-hemo38', 'f3fa-hene44', 'f3fa-heno70', 'f3fa-hera849', 'f3fa-heso89', 'f3fa-hete722', 'f3fa-heti782', 'f3fa-heze61', 'f3fa-hiba14', 'f3fa-hiba275', 'f3fa-hido53', 'f3fa-higy53', 'f3fa-hije723', 'f3fa-hika56', 'f3fa-hike09', 'f3fa-hima59', 'f3fa-hime87', 'f3fa-himo77', 'f3fa-hinu75', 'f3fa-hiqe06', 'f3fa-hiqi193', 'f3fa-hiqu77', 'f3fa-hisi80', 'f3fa-hite71', 'f3fa-hito78', 'f3fa-hivo89', 'f3fa-hizi595', 'f3fa-hobi07', 'f3fa-hobo56', 'f3fa-hoby62', 'f3fa-hocy542', 'f3fa-hofu54', 'f3fa-hoha69', 'f3fa-hoje57', 'f3fa-hoku53', 'f3fa-home05', 'f3fa-homo33', 'f3fa-hona55', 'f3fa-hono075', 'f3fa-hopu99', 'f3fa-hora99', 'f3fa-horo98', 'f3fa-hosi047', 'f3fa-hoti24', 'f3fa-hova74', 'f3fa-hoza47', 'f3fa-huco61', 'f3fa-hucu55', 'f3fa-hufu94', 'f3fa-hugi17', 'f3fa-hugu746', 'f3fa-huju232', 'f3fa-hunu824', 'f3fa-huqa763', 'f3fa-huqa78', 'f3fa-huqe26', 'f3fa-husa01', 'f3fa-husa25', 'f3fa-huso29', 'f3fa-husy702', 'f3fa-huvy85', 'f3fa-huxi872', 'f3fa-huzy761', 'f3fa-hyba936', 'f3fa-hyca733', 'f3fa-hydi57', 'f3fa-hyfe86', 'f3fa-hyja716', 'f3fa-hymu510', 'f3fa-hyqe697', 'f3fa-hyqu611', 'f3fa-hyro469', 'f3fa-hysu40', 'f3fa-hyvu110', 'f3fa-hyvu97', 'f3fa-hyxo71', 'f3fa-hyze112', 'f3fa-hyzo29', 'f3fa-hyzy658', 'f3fa-jabo771', 'f3fa-jaca894', 'f3fa-jada580', 'f3fa-jade46', 'f3fa-jafu12', 'f3fa-jago23', 'f3fa-jahi318', 'f3fa-jaja65', 'f3fa-jaje65', 'f3fa-jaji09', 'f3fa-jaji67', 'f3fa-jala57', 'f3fa-jalo29', 'f3fa-jaly20', 'f3fa-jame574', 'f3fa-jami32', 'f3fa-jany066', 'f3fa-jasa989', 'f3fa-jaty840', 'f3fa-jaza49', 'f3fa-jazi164', 'f3fa-jazo28', 'f3fa-jazo30', 'f3fa-jedi630', 'f3fa-jega01', 'f3fa-jegy28', 'f3fa-jehi16', 'f3fa-jeho19', 'f3fa-jeho89', 'f3fa-jehu27', 'f3fa-jejo469', 'f3fa-jejy23', 'f3fa-jeli81', 'f3fa-jemu62', 'f3fa-jene78', 'f3fa-jeqo54', 'f3fa-jeqy61', 'f3fa-jeru15', 'f3fa-jery20', 'f3fa-jesi560', 'f3fa-jexi636', 'f3fa-jezi22', 'f3fa-jiba29', 'f3fa-jici83', 'f3fa-jicy166', 'f3fa-jife07', 'f3fa-jigy002', 'f3fa-jile860', 'f3fa-jima32', 'f3fa-jimo59', 'f3fa-jina210', 'f3fa-jiri139', 'f3fa-jiri35', 'f3fa-jiry069', 'f3fa-jiso870', 'f3fa-jixo916', 'f3fa-jobu29', 'f3fa-joca89', 'f3fa-joci47', 'f3fa-jocy13', 'f3fa-jodi05', 'f3fa-johe076', 'f3fa-johe37', 'f3fa-johi814', 'f3fa-jona44', 'f3fa-jopy74', 'f3fa-joqo38', 'f3fa-joqo71', 'f3fa-joqu903', 'f3fa-joru22', 'f3fa-joso61', 'f3fa-joty94', 'f3fa-jovu510', 'f3fa-joza39', 'f3fa-jozo06', 'f3fa-jubo178', 'f3fa-jubu77', 'f3fa-jucu74', 'f3fa-jufi916', 'f3fa-jufy17', 'f3fa-jugy073', 'f3fa-juhu79', 'f3fa-juhy85', 'f3fa-juje39', 'f3fa-jule86', 'f3fa-junu36', 'f3fa-jupy854', 'f3fa-juqe87', 'f3fa-juqy29', 'f3fa-juri70', 'f3fa-juxi25', 'f3fa-jyco18', 'f3fa-jydu33', 'f3fa-jyhi430', 'f3fa-jyky81', 'f3fa-jyny199', 'f3fa-jyso30', 'f3fa-jyve33', 'f3fa-jyzo277', 'f3fa-kaba08', 'f3fa-kaci953', 'f3fa-kadi22', 'f3fa-kaga104', 'f3fa-kaga977', 'f3fa-kagi98', 'f3fa-kani73', 'f3fa-kapu16', 'f3fa-kaqo310', 'f3fa-kara91', 'f3fa-kare50', 'f3fa-kasa846', 'f3fa-kasi29', 'f3fa-kasi36', 'f3fa-kati316', 'f3fa-kato492', 'f3fa-kave902', 'f3fa-kazi00', 'f3fa-keca10', 'f3fa-keca636', 'f3fa-kedo70', 'f3fa-kefu77', 'f3fa-keji195', 'f3fa-kele96', 'f3fa-keli00', 'f3fa-kelo32', 'f3fa-kenu228', 'f3fa-kenu804', 'f3fa-keri181', 'f3fa-kete97', 'f3fa-keve35', 'f3fa-kexu85', 'f3fa-kexy160', 'f3fa-keze800', 'f3fa-kibi013', 'f3fa-kidi45', 'f3fa-kifa15', 'f3fa-kigi12', 'f3fa-kigy01', 'f3fa-kigy537', 'f3fa-kiny65', 'f3fa-kiqy337', 'f3fa-kira74', 'f3fa-kira86', 'f3fa-kire173', 'f3fa-kire38', 'f3fa-kiro01', 'f3fa-kiro53', 'f3fa-kisi370', 'f3fa-kiti34', 'f3fa-kiti85', 'f3fa-kivu48', 'f3fa-kixy11', 'f3fa-kizo31', 'f3fa-kobi10', 'f3fa-kobu04', 'f3fa-kocu85', 'f3fa-koga48', 'f3fa-koli24', 'f3fa-koli28', 'f3fa-kore767', 'f3fa-kote10', 'f3fa-koxa25', 'f3fa-koxa72', 'f3fa-koxo331', 'f3fa-koxo676', 'f3fa-koxy91', 'f3fa-koza917', 'f3fa-kuby44', 'f3fa-kuco85', 'f3fa-kucu49', 'f3fa-kuhe86', 'f3fa-kuko77', 'f3fa-kune115', 'f3fa-kupe58', 'f3fa-kuqe649', 'f3fa-kuqu90', 'f3fa-kusi45', 'f3fa-kusu904', 'f3fa-kusy307', 'f3fa-kuta89', 'f3fa-kuti11', 'f3fa-kuto24', 'f3fa-kuty22', 'f3fa-kuvu54', 'f3fa-kuxo046', 'f3fa-kybu47', 'f3fa-kyca83', 'f3fa-kyce85', 'f3fa-kyci386', 'f3fa-kyda247', 'f3fa-kygo54', 'f3fa-kyja227', 'f3fa-kyju60', 'f3fa-kyki64', 'f3fa-kymo001', 'f3fa-kymu06', 'f3fa-kynu02', 'f3fa-kypi06', 'f3fa-kyre83', 'f3fa-kysa84', 'f3fa-kyti33', 'f3fa-kyxi81', 'f3fa-labi00', 'f3fa-laca37', 'f3fa-laca55', 'f3fa-laco88', 'f3fa-lacu08', 'f3fa-lacy50', 'f3fa-lado744', 'f3fa-lady628', 'f3fa-lafi95', 'f3fa-laja554', 'f3fa-lama23', 'f3fa-lanu59', 'f3fa-lapi04', 'f3fa-laqi52', 'f3fa-lari84', 'f3fa-lase159', 'f3fa-lasy53', 'f3fa-lati33', 'f3fa-laxi257', 'f3fa-laxy16', 'f3fa-lazo058', 'f3fa-lebu78', 'f3fa-ledu97', 'f3fa-ledy27', 'f3fa-ledy43', 'f3fa-lefy63', 'f3fa-lefy832', 'f3fa-lege29', 'f3fa-legi82', 'f3fa-leha48', 'f3fa-leja857', 'f3fa-leje62', 'f3fa-leki73', 'f3fa-leli93', 'f3fa-leny12', 'f3fa-lepe60', 'f3fa-leqe77', 'f3fa-leqy75', 'f3fa-lera30', 'f3fa-lery912', 'f3fa-lete99', 'f3fa-leva46', 'f3fa-levu61', 'f3fa-libu78', 'f3fa-lice06', 'f3fa-lide30', 'f3fa-lidu288', 'f3fa-lidu73', 'f3fa-lifo75', 'f3fa-lifu75', 'f3fa-lige215', 'f3fa-lige71', 'f3fa-ligy517', 'f3fa-liha95', 'f3fa-lihu92', 'f3fa-liji92', 'f3fa-like54', 'f3fa-liko70', 'f3fa-lile83', 'f3fa-lino328', 'f3fa-liro01', 'f3fa-liso99', 'f3fa-lite33', 'f3fa-lity361', 'f3fa-lixi557', 'f3fa-lixu716', 'f3fa-liza19', 'f3fa-lizi60', 'f3fa-lizu30', 'f3fa-lobu49', 'f3fa-loci692', 'f3fa-lode212', 'f3fa-loga76', 'f3fa-loge226', 'f3fa-loge97', 'f3fa-lone959', 'f3fa-lope749', 'f3fa-lopo87', 'f3fa-loru63', 'f3fa-lovi76', 'f3fa-lovi89', 'f3fa-loxi964', 'f3fa-loxo14', 'f3fa-loxy955', 'f3fa-luba337', 'f3fa-luby970', 'f3fa-ludo80', 'f3fa-ludu33', 'f3fa-lugu93', 'f3fa-luha90', 'f3fa-luje30', 'f3fa-luky04', 'f3fa-lumi503', 'f3fa-lune59', 'f3fa-lupo307', 'f3fa-lure14', 'f3fa-luri718', 'f3fa-lusa96', 'f3fa-lusy105', 'f3fa-luto99', 'f3fa-lydi016', 'f3fa-lydo43', 'f3fa-lydu68', 'f3fa-lyga36', 'f3fa-lyho91', 'f3fa-lyjy99', 'f3fa-lyko667', 'f3fa-lyky28', 'f3fa-lylu80', 'f3fa-lyme84', 'f3fa-lymo88', 'f3fa-lyny512', 'f3fa-lyqa99', 'f3fa-lyre48', 'f3fa-lyte067', 'f3fa-lyti70', 'f3fa-lyvo37', 'f3fa-lyzi509', 'f3fa-mabe64', 'f3fa-mabu63', 'f3fa-mace83', 'f3fa-maco002', 'f3fa-mafo039', 'f3fa-mago84', 'f3fa-maje075', 'f3fa-mapa69', 'f3fa-maqi32', 'f3fa-mara779', 'f3fa-mari64', 'f3fa-mate052', 'f3fa-mava564', 'f3fa-mavu411', 'f3fa-maxy530', 'f3fa-mazi575', 'f3fa-mazu72', 'f3fa-meda98', 'f3fa-medo97', 'f3fa-medy46', 'f3fa-mefe54', 'f3fa-mefy43', 'f3fa-meka98', 'f3fa-meko20', 'f3fa-meku405', 'f3fa-mela34', 'f3fa-mele07', 'f3fa-melo12', 'f3fa-mepe72', 'f3fa-mepe91', 'f3fa-mesi117', 'f3fa-mete617', 'f3fa-meti49', 'f3fa-mevy14', 'f3fa-mevy28', 'f3fa-mezi62', 'f3fa-mezu20', 'f3fa-mibi26', 'f3fa-mibu74', 'f3fa-mida61', 'f3fa-mide075', 'f3fa-mido13', 'f3fa-mifa33', 'f3fa-mife41', 'f3fa-mife74', 'f3fa-mify92', 'f3fa-mige78', 'f3fa-migy40', 'f3fa-mihy91', 'f3fa-mije474', 'f3fa-mijo284', 'f3fa-miko37', 'f3fa-miku19', 'f3fa-miky28', 'f3fa-miky79', 'f3fa-mira157', 'f3fa-miru13', 'f3fa-misi34', 'f3fa-miti66', 'f3fa-miti853', 'f3fa-mivy35', 'f3fa-mivy43', 'f3fa-mixu268', 'f3fa-mixu82', 'f3fa-mixy23', 'f3fa-mixy94', 'f3fa-mize13', 'f3fa-mizi32', 'f3fa-mizu223', 'f3fa-mizu58', 'f3fa-moby38', 'f3fa-mode65', 'f3fa-modi03', 'f3fa-mofa33', 'f3fa-mofu601', 'f3fa-mogy35', 'f3fa-mole735', 'f3fa-mone01', 'f3fa-monu78', 'f3fa-mory65', 'f3fa-mote36', 'f3fa-movi431', 'f3fa-moxe67', 'f3fa-muda43', 'f3fa-muda80', 'f3fa-mudi48', 'f3fa-muga86', 'f3fa-muha37', 'f3fa-muki233', 'f3fa-mula60', 'f3fa-muli226', 'f3fa-muna988', 'f3fa-muni32', 'f3fa-mupa452', 'f3fa-muta53', 'f3fa-muzo840', 'f3fa-muzu35', 'f3fa-mybu86', 'f3fa-myco20', 'f3fa-myda62', 'f3fa-mydo20', 'f3fa-myfa459', 'f3fa-mygu492', 'f3fa-myhu27', 'f3fa-mymo296', 'f3fa-mymy02', 'f3fa-myna39', 'f3fa-mynu338', 'f3fa-mypi64', 'f3fa-myra370', 'f3fa-mysa192', 'f3fa-mysa78', 'f3fa-mysi12', 'f3fa-myta74', 'f3fa-myti26', 'f3fa-myti356', 'f3fa-myzi202', 'f3fa-myzu90', 'f3fa-naba18', 'f3fa-nace57', 'f3fa-nade18', 'f3fa-nadu22', 'f3fa-nafa192', 'f3fa-nahi081', 'f3fa-nahy30', 'f3fa-nake74', 'f3fa-naku756', 'f3fa-namo74', 'f3fa-nana41', 'f3fa-nape45', 'f3fa-napu46', 'f3fa-nare48', 'f3fa-natu38', 'f3fa-nava82', 'f3fa-navu10', 'f3fa-naxi78', 'f3fa-naxu530', 'f3fa-naza227', 'f3fa-neba96', 'f3fa-nece09', 'f3fa-necu26', 'f3fa-necy54', 'f3fa-negi02', 'f3fa-nehe19', 'f3fa-nehe80', 'f3fa-neky11', 'f3fa-neqo27', 'f3fa-nero382', 'f3fa-neta72', 'f3fa-neto579', 'f3fa-neto744', 'f3fa-nevi058', 'f3fa-nicu01', 'f3fa-nidu26', 'f3fa-nife27', 'f3fa-nife40', 'f3fa-nife961', 'f3fa-niji78', 'f3fa-nijy83', 'f3fa-nili347', 'f3fa-nily19', 'f3fa-nime64', 'f3fa-nimy60', 'f3fa-niro55', 'f3fa-nitu83', 'f3fa-nity955', 'f3fa-niva009', 'f3fa-nive61', 'f3fa-nive975', 'f3fa-nixa67', 'f3fa-nobe948', 'f3fa-noby17', 'f3fa-noce19', 'f3fa-nocu69', 'f3fa-nodi58', 'f3fa-nody86', 'f3fa-nofu06', 'f3fa-noha02', 'f3fa-noje438', 'f3fa-nomi21', 'f3fa-nona91', 'f3fa-noni524', 'f3fa-nony79', 'f3fa-nopy061', 'f3fa-noqa89', 'f3fa-nory64', 'f3fa-nosu69', 'f3fa-nove77', 'f3fa-novu109', 'f3fa-noxe55', 'f3fa-noxi04', 'f3fa-noxi41', 'f3fa-nozo65', 'f3fa-nozu42', 'f3fa-nubo67', 'f3fa-nuby93', 'f3fa-nuda41', 'f3fa-nudo89', 'f3fa-nudu885', 'f3fa-nugo43', 'f3fa-nuji529', 'f3fa-nuka65', 'f3fa-nuke75', 'f3fa-nuky199', 'f3fa-numy100', 'f3fa-nunu756', 'f3fa-nupu38', 'f3fa-nupy02', 'f3fa-nuri804', 'f3fa-nuro90', 'f3fa-nute242', 'f3fa-nuti050', 'f3fa-nuva451', 'f3fa-nyco27', 'f3fa-nycu98', 'f3fa-nyda42', 'f3fa-nydi50', 'f3fa-nyfy632', 'f3fa-nyga22', 'f3fa-nyge65', 'f3fa-nyhe929', 'f3fa-nyho234', 'f3fa-nyho276', 'f3fa-nyhy34', 'f3fa-nyje18', 'f3fa-nyke97', 'f3fa-nyki31', 'f3fa-nyko36', 'f3fa-nyma540', 'f3fa-nypo492', 'f3fa-nypy430', 'f3fa-nyqy900', 'f3fa-nyry43', 'f3fa-nysy36', 'f3fa-nyva49', 'f3fa-nyve35', 'f3fa-nyve870', 'f3fa-nyza27', 'f3fa-nyzi671', 'f3fa-paci18', 'f3fa-pacu660', 'f3fa-padu28', 'f3fa-pajy29', 'f3fa-pake58', 'f3fa-pako502', 'f3fa-palo82', 'f3fa-pami09', 'f3fa-pamo62', 'f3fa-pamy82', 'f3fa-pano84', 'f3fa-pany75', 'f3fa-papi238', 'f3fa-paru21', 'f3fa-pave10', 'f3fa-paxi969', 'f3fa-pebi82', 'f3fa-pedi12', 'f3fa-pedy28', 'f3fa-pege84', 'f3fa-pego133', 'f3fa-peha45', 'f3fa-peke15', 'f3fa-peli09', 'f3fa-pelo959', 'f3fa-pemy49', 'f3fa-pesi47', 'f3fa-peti24', 'f3fa-peti805', 'f3fa-peve12', 'f3fa-pevi835', 'f3fa-pevo77', 'f3fa-pexi60', 'f3fa-peza38', 'f3fa-pibu339', 'f3fa-pibu64', 'f3fa-pice85', 'f3fa-pida50', 'f3fa-pidu57', 'f3fa-pidy920', 'f3fa-pifa25', 'f3fa-pife41', 'f3fa-pifu15', 'f3fa-pifu35', 'f3fa-pifu42', 'f3fa-pige077', 'f3fa-pige11', 'f3fa-pija54', 'f3fa-pije46', 'f3fa-pije619', 'f3fa-pinu70', 'f3fa-piqi43', 'f3fa-pobi55', 'f3fa-poby25', 'f3fa-podi00', 'f3fa-podu014', 'f3fa-pofi56', 'f3fa-poje425', 'f3fa-pojo26', 'f3fa-poju952', 'f3fa-polo81', 'f3fa-poma69', 'f3fa-pomi027', 'f3fa-pori51', 'f3fa-poti73', 'f3fa-poto77', 'f3fa-poxi32', 'f3fa-poxu53', 'f3fa-pozo93', 'f3fa-puge675', 'f3fa-pume01', 'f3fa-pumi03', 'f3fa-pumi88', 'f3fa-pumy76', 'f3fa-puno63', 'f3fa-pupi48', 'f3fa-pupo692', 'f3fa-pupy65', 'f3fa-puqo388', 'f3fa-puse51', 'f3fa-puse68', 'f3fa-pusi50', 'f3fa-puta98', 'f3fa-putu334', 'f3fa-puvu13', 'f3fa-puxa45', 'f3fa-puze02', 'f3fa-puzo068', 'f3fa-puzo230', 'f3fa-puzy338', 'f3fa-pycy127', 'f3fa-pyda71', 'f3fa-pydo80', 'f3fa-pyhe219', 'f3fa-pyho15', 'f3fa-pyle12', 'f3fa-pymu090', 'f3fa-pymu88', 'f3fa-pyna77', 'f3fa-pypo881', 'f3fa-pyta23', 'f3fa-pyza89', 'f3fa-pyzu26', 'f3fa-qabe11', 'f3fa-qaby535', 'f3fa-qaca07', 'f3fa-qaco159', 'f3fa-qade98', 'f3fa-qafo28', 'f3fa-qagi459', 'f3fa-qagy552', 'f3fa-qaha79', 'f3fa-qaho52', 'f3fa-qajy86', 'f3fa-qamo99', 'f3fa-qamu609', 'f3fa-qamu86', 'f3fa-qana33', 'f3fa-qani30', 'f3fa-qapi49', 'f3fa-qapo649', 'f3fa-qasi86', 'f3fa-qaty738', 'f3fa-qava97', 'f3fa-qavo104', 'f3fa-qefe70', 'f3fa-qega045', 'f3fa-qehi62', 'f3fa-qeka895', 'f3fa-qeku841', 'f3fa-qela380', 'f3fa-qemi97', 'f3fa-qemi98', 'f3fa-qemy17', 'f3fa-qepe391', 'f3fa-qeqe544', 'f3fa-qera18', 'f3fa-qesi43', 'f3fa-qetu73', 'f3fa-qety416', 'f3fa-qevy85', 'f3fa-qexa72', 'f3fa-qeza31', 'f3fa-qibo858', 'f3fa-qica44', 'f3fa-qice17', 'f3fa-qifu12', 'f3fa-qifu54', 'f3fa-qiha800', 'f3fa-qihi26', 'f3fa-qije82', 'f3fa-qijo78', 'f3fa-qima59', 'f3fa-qimu90', 'f3fa-qimy624', 'f3fa-qina33', 'f3fa-qine15', 'f3fa-qinu475', 'f3fa-qiqa006', 'f3fa-qira618', 'f3fa-qixe39', 'f3fa-qixi89', 'f3fa-qiza89', 'f3fa-qize536', 'f3fa-qocu28', 'f3fa-qocy073', 'f3fa-qocy54', 'f3fa-qodi729', 'f3fa-qogo78', 'f3fa-qohe583', 'f3fa-qoho59', 'f3fa-qomi94', 'f3fa-qomo20', 'f3fa-qomo55', 'f3fa-qomy97', 'f3fa-qone842', 'f3fa-qono767', 'f3fa-qoqo065', 'f3fa-qove33', 'f3fa-qovi61', 'f3fa-qoxe657', 'f3fa-qoxy539', 'f3fa-qozu95', 'f3fa-quca892', 'f3fa-quce512', 'f3fa-quco22', 'f3fa-qucu147', 'f3fa-quhy946', 'f3fa-quji05', 'f3fa-quku39', 'f3fa-quky53', 'f3fa-quma18', 'f3fa-qumy745', 'f3fa-qupa74', 'f3fa-qupo65', 'f3fa-qupo76', 'f3fa-quqi37', 'f3fa-quxu545', 'f3fa-qyby543', 'f3fa-qyce44', 'f3fa-qydu27', 'f3fa-qyfi14', 'f3fa-qyho94', 'f3fa-qyki27', 'f3fa-qyki392', 'f3fa-qyku29', 'f3fa-qylu068', 'f3fa-qype02', 'f3fa-qyqi57', 'f3fa-qyqu65', 'f3fa-qyqy89', 'f3fa-qyra96', 'f3fa-qysi039', 'f3fa-qysy143', 'f3fa-qyti63', 'f3fa-qyve48', 'f3fa-qyza98', 'f3fa-qyzi351', 'f3fa-raba28', 'f3fa-rabi25', 'f3fa-rabo68', 'f3fa-rabu35', 'f3fa-racu79', 'f3fa-rada070', 'f3fa-rada18', 'f3fa-rade043', 'f3fa-ragu00', 'f3fa-rale14', 'f3fa-ralo65', 'f3fa-raly66', 'f3fa-ramo86', 'f3fa-ramu54', 'f3fa-rana37', 'f3fa-rane400', 'f3fa-ranu37', 'f3fa-rasa93', 'f3fa-ratu538', 'f3fa-rede43', 'f3fa-redy731', 'f3fa-reje729', 'f3fa-rejo40', 'f3fa-rejy922', 'f3fa-reka24', 'f3fa-reke65', 'f3fa-reku79', 'f3fa-rele46', 'f3fa-remy26', 'f3fa-repi69', 'f3fa-requ05', 'f3fa-reru320', 'f3fa-resi44', 'f3fa-resu94', 'f3fa-revo601', 'f3fa-reze681', 'f3fa-rezi16', 'f3fa-rici51', 'f3fa-ridu20', 'f3fa-rifu370', 'f3fa-rigi221', 'f3fa-riho96', 'f3fa-rije82', 'f3fa-riqa627', 'f3fa-riqi99', 'f3fa-riqy43', 'f3fa-rire09', 'f3fa-riso16', 'f3fa-riso80', 'f3fa-risy72', 'f3fa-rizu947', 'f3fa-roda99', 'f3fa-rodu18', 'f3fa-rofe44', 'f3fa-rogi030', 'f3fa-rojo069', 'f3fa-roku49', 'f3fa-roku90', 'f3fa-roli965', 'f3fa-rolo690', 'f3fa-rome381', 'f3fa-romu34', 'f3fa-rony16', 'f3fa-roro34', 'f3fa-rosa46', 'f3fa-rotu13', 'f3fa-rova793', 'f3fa-rube98', 'f3fa-ruca41', 'f3fa-rufi45', 'f3fa-rugy115', 'f3fa-ruhi763', 'f3fa-ruhi77', 'f3fa-ruke31', 'f3fa-ruke95', 'f3fa-ruko07', 'f3fa-rumo23', 'f3fa-rumu05', 'f3fa-runo307', 'f3fa-rupa12', 'f3fa-rupa672', 'f3fa-ruro12', 'f3fa-rury06', 'f3fa-ruti65', 'f3fa-ruvy71', 'f3fa-ruzy84', 'f3fa-rybe81', 'f3fa-ryce65', 'f3fa-ryco69', 'f3fa-ryco865', 'f3fa-rycu62', 'f3fa-ryde06', 'f3fa-ryho81', 'f3fa-ryko33', 'f3fa-rylu025', 'f3fa-ryma10', 'f3fa-ryme35', 'f3fa-ryny36', 'f3fa-rypu69', 'f3fa-ryse348', 'f3fa-ryso188', 'f3fa-ryza587', 'f3fa-ryzi15', 'f3fa-saci17', 'f3fa-saci50', 'f3fa-sacy44', 'f3fa-safe101', 'f3fa-saga64', 'f3fa-saje33', 'f3fa-saku84', 'f3fa-saky39', 'f3fa-saky79', 'f3fa-sala481', 'f3fa-saly19', 'f3fa-saqi56', 'f3fa-saqu39', 'f3fa-saro40', 'f3fa-sasi47', 'f3fa-sasu060', 'f3fa-sato30', 'f3fa-save14', 'f3fa-sazi52', 'f3fa-sebe702', 'f3fa-seco33', 'f3fa-secu84', 'f3fa-secy655', 'f3fa-sefa10', 'f3fa-sego89', 'f3fa-sehe41', 'f3fa-sehi92', 'f3fa-seho95', 'f3fa-seji873', 'f3fa-seno04', 'f3fa-seny23', 'f3fa-seny620', 'f3fa-sepi224', 'f3fa-seqo732', 'f3fa-sesa44', 'f3fa-sesi34', 'f3fa-sesu405', 'f3fa-sete40', 'f3fa-seti15', 'f3fa-setu25', 'f3fa-sevy138', 'f3fa-sexy06', 'f3fa-sezu596', 'f3fa-sibu33', 'f3fa-side56', 'f3fa-sido706', 'f3fa-sidy80', 'f3fa-sifu69', 'f3fa-siga218', 'f3fa-sihu782', 'f3fa-siju570', 'f3fa-sijy441', 'f3fa-sila50', 'f3fa-sila69', 'f3fa-sime24', 'f3fa-simy04', 'f3fa-siny22', 'f3fa-siny39', 'f3fa-sipi68', 'f3fa-sipy320', 'f3fa-sipy579', 'f3fa-siqa19', 'f3fa-sira458', 'f3fa-siso52', 'f3fa-siva72', 'f3fa-sixo99', 'f3fa-sixy15', 'f3fa-sizy63', 'f3fa-sobo96', 'f3fa-soce26', 'f3fa-soce997', 'f3fa-sode612', 'f3fa-sofo51', 'f3fa-sogi67', 'f3fa-sogu15', 'f3fa-sohy22', 'f3fa-soli579', 'f3fa-soly88', 'f3fa-soma618', 'f3fa-somu22', 'f3fa-sonu45', 'f3fa-sony95', 'f3fa-sopo67', 'f3fa-soqe61', 'f3fa-soqo52', 'f3fa-sori06', 'f3fa-sota77', 'f3fa-soti783', 'f3fa-soxe178', 'f3fa-soxe75', 'f3fa-sozu564', 'f3fa-suce17', 'f3fa-sufa02', 'f3fa-sufe50', 'f3fa-sufy50', 'f3fa-sugi385', 'f3fa-sugy705', 'f3fa-suhe21', 'f3fa-sume31', 'f3fa-sumo936', 'f3fa-suro240', 'f3fa-suvo86', 'f3fa-suxi10', 'f3fa-suzy06', 'f3fa-syca14', 'f3fa-syco77', 'f3fa-syda40', 'f3fa-syde26', 'f3fa-sydi14', 'f3fa-syfi57', 'f3fa-syfy62', 'f3fa-syje27', 'f3fa-syje99', 'f3fa-syjo64', 'f3fa-syku536', 'f3fa-syky77', 'f3fa-syni79', 'f3fa-syno714', 'f3fa-syny03', 'f3fa-syry663', 'f3fa-syvi14', 'f3fa-syvo070', 'f3fa-syza76', 'f3fa-syze870', 'f3fa-tafo073', 'f3fa-tafo23', 'f3fa-tage62', 'f3fa-tagu49', 'f3fa-taha35', 'f3fa-taju53', 'f3fa-taka73', 'f3fa-taki077', 'f3fa-taky14', 'f3fa-talo08', 'f3fa-tami554', 'f3fa-tamy47', 'f3fa-tapu537', 'f3fa-tary59', 'f3fa-tata29', 'f3fa-tati36', 'f3fa-tavu24', 'f3fa-taxa33', 'f3fa-teby29', 'f3fa-tedu28', 'f3fa-tefa762', 'f3fa-tefu89', 'f3fa-teji85', 'f3fa-tejy57', 'f3fa-tepi26', 'f3fa-tepu10', 'f3fa-tequ080', 'f3fa-tere15', 'f3fa-teri29', 'f3fa-teri77', 'f3fa-tesy85', 'f3fa-teta99', 'f3fa-tevi994', 'f3fa-texa07', 'f3fa-tibe590', 'f3fa-tice35', 'f3fa-tife35', 'f3fa-tifu085', 'f3fa-tify716', 'f3fa-tige064', 'f3fa-tije725', 'f3fa-tiju246', 'f3fa-tijy15', 'f3fa-tilo44', 'f3fa-time013', 'f3fa-tipi006', 'f3fa-tiri60', 'f3fa-tite99', 'f3fa-tiza79', 'f3fa-tizi792', 'f3fa-toci28', 'f3fa-tocu851', 'f3fa-tocy894', 'f3fa-todo72', 'f3fa-tofy168', 'f3fa-toku57', 'f3fa-toky695', 'f3fa-tola10', 'f3fa-tona62', 'f3fa-toqy64', 'f3fa-tore165', 'f3fa-toru008', 'f3fa-tosi09', 'f3fa-tote776', 'f3fa-toto30', 'f3fa-toty868', 'f3fa-tovo13', 'f3fa-toze08', 'f3fa-tube483', 'f3fa-tubi432', 'f3fa-tuho00', 'f3fa-tuhy701', 'f3fa-tuje909', 'f3fa-tupe48', 'f3fa-tupi13', 'f3fa-tupu85', 'f3fa-tury02', 'f3fa-tuse52', 'f3fa-tuty90', 'f3fa-tuvy896', 'f3fa-tuzo16', 'f3fa-tuzy42', 'f3fa-tycu600', 'f3fa-tydy180', 'f3fa-tyfy53', 'f3fa-tyga41', 'f3fa-tygo660', 'f3fa-tyhu30', 'f3fa-tyka22', 'f3fa-tyla29', 'f3fa-tyli039', 'f3fa-tyli545', 'f3fa-tymi216', 'f3fa-tymo99', 'f3fa-tyne46', 'f3fa-tyqu730', 'f3fa-tyve67', 'f3fa-tyxe75', 'f3fa-tyxi88', 'f3fa-tyzi516', 'f3fa-vabo908', 'f3fa-vace37', 'f3fa-vady28', 'f3fa-vamu12', 'f3fa-vamy14', 'f3fa-vaqo15', 'f3fa-vaqo56', 'f3fa-vasa96', 'f3fa-vasu827', 'f3fa-vatu03', 'f3fa-vatu29', 'f3fa-vaxu40', 'f3fa-vebi47', 'f3fa-vebo312', 'f3fa-vefo90', 'f3fa-vegi31', 'f3fa-veho129', 'f3fa-vela816', 'f3fa-velo14', 'f3fa-velo47', 'f3fa-veno54', 'f3fa-veri47', 'f3fa-vesu03', 'f3fa-vesy02', 'f3fa-vesy66', 'f3fa-veti175', 'f3fa-vevy37', 'f3fa-veze368', 'f3fa-vezu31', 'f3fa-vicu33', 'f3fa-vido933', 'f3fa-vidy563', 'f3fa-viha27', 'f3fa-vihu34', 'f3fa-vike12', 'f3fa-viko414', 'f3fa-vipo62', 'f3fa-vipo93', 'f3fa-vipu07', 'f3fa-viqa46', 'f3fa-viqo14', 'f3fa-viru12', 'f3fa-viso53', 'f3fa-vita47', 'f3fa-vivy671', 'f3fa-vixi037', 'f3fa-vizy83', 'f3fa-voce04', 'f3fa-voda39', 'f3fa-vofo03', 'f3fa-vofo82', 'f3fa-vogy68', 'f3fa-voha664', 'f3fa-vojo685', 'f3fa-voka388', 'f3fa-voko07', 'f3fa-volu66', 'f3fa-vomy09', 'f3fa-vopo05', 'f3fa-voru63', 'f3fa-vose53', 'f3fa-voso79', 'f3fa-voso94', 'f3fa-vosy69', 'f3fa-voto29', 'f3fa-voxe067', 'f3fa-voze02', 'f3fa-vozu83', 'f3fa-vuco549', 'f3fa-vudi00', 'f3fa-vudi23', 'f3fa-vudi98', 'f3fa-vufu52', 'f3fa-vuhy93', 'f3fa-vuje285', 'f3fa-vuju29', 'f3fa-vujy066', 'f3fa-vuka73', 'f3fa-vuka850', 'f3fa-vuky52', 'f3fa-vume15', 'f3fa-vumo42', 'f3fa-vuqo00', 'f3fa-vuri83', 'f3fa-vury79', 'f3fa-vuve83', 'f3fa-vuxa04', 'f3fa-vuxo480', 'f3fa-vuzo36', 'f3fa-vybu350', 'f3fa-vyca132', 'f3fa-vyco859', 'f3fa-vyde95', 'f3fa-vyfa665', 'f3fa-vyhy51', 'f3fa-vyhy72', 'f3fa-vyji492', 'f3fa-vylo32', 'f3fa-vyly23', 'f3fa-vyme91', 'f3fa-vymu38', 'f3fa-vynu957', 'f3fa-vypo36', 'f3fa-vypo47', 'f3fa-vyqo11', 'f3fa-vysy67', 'f3fa-vyti94', 'f3fa-vyva207', 'f3fa-vyve255', 'f3fa-vyzy28', 'f3fa-xabe580', 'f3fa-xaco15', 'f3fa-xafa667', 'f3fa-xagi134', 'f3fa-xaho23', 'f3fa-xaho64', 'f3fa-xako47', 'f3fa-xana61', 'f3fa-xanu29', 'f3fa-xaqi01', 'f3fa-xaqo58', 'f3fa-xaqu59', 'f3fa-xare65', 'f3fa-xari869', 'f3fa-xary78', 'f3fa-xase51', 'f3fa-xasy237', 'f3fa-xaty65', 'f3fa-xava117', 'f3fa-xaza685', 'f3fa-xazi78', 'f3fa-xebi75', 'f3fa-xefa26', 'f3fa-xega94', 'f3fa-xeha27', 'f3fa-xehe585', 'f3fa-xehe74', 'f3fa-xeki46', 'f3fa-xela75', 'f3fa-xema043', 'f3fa-xema552', 'f3fa-xemy65', 'f3fa-xeni396', 'f3fa-xeqe55', 'f3fa-xete322', 'f3fa-xeve55', 'f3fa-xevu796', 'f3fa-xexa57', 'f3fa-xezo784', 'f3fa-xezy252', 'f3fa-xezy53', 'f3fa-xibe58', 'f3fa-xico83', 'f3fa-xida97', 'f3fa-xifo424', 'f3fa-xija82', 'f3fa-xijo534', 'f3fa-xila54', 'f3fa-xile427', 'f3fa-ximu91', 'f3fa-xipa81', 'f3fa-xipi45', 'f3fa-xiqa48', 'f3fa-xiqi79', 'f3fa-xiqy17', 'f3fa-xiru24', 'f3fa-xiry56', 'f3fa-xixe01', 'f3fa-xixe553', 'f3fa-xiza522', 'f3fa-xocy367', 'f3fa-xodi792', 'f3fa-xogy76', 'f3fa-xohy97', 'f3fa-xoja833', 'f3fa-xomu096', 'f3fa-xone82', 'f3fa-xoni32', 'f3fa-xoni958', 'f3fa-xopo20', 'f3fa-xoru86', 'f3fa-xory52', 'f3fa-xose04', 'f3fa-xosu429', 'f3fa-xoto33', 'f3fa-xotu251', 'f3fa-xovu78', 'f3fa-xoxu36', 'f3fa-xozi94', 'f3fa-xucu15', 'f3fa-xufi89', 'f3fa-xufo13', 'f3fa-xuka899', 'f3fa-xule961', 'f3fa-xuna05', 'f3fa-xune13', 'f3fa-xupo121', 'f3fa-xuqu65', 'f3fa-xuro60', 'f3fa-xuto07', 'f3fa-xuvo73', 'f3fa-xuvo74', 'f3fa-xuxo03', 'f3fa-xuxo927', 'f3fa-xuze89', 'f3fa-xyby79', 'f3fa-xydo22', 'f3fa-xydo955', 'f3fa-xydu572', 'f3fa-xydy47', 'f3fa-xydy88', 'f3fa-xyhu77', 'f3fa-xyhy378', 'f3fa-xyja027', 'f3fa-xyju11', 'f3fa-xyka34', 'f3fa-xymo85', 'f3fa-xyny828', 'f3fa-xype10', 'f3fa-xysa56', 'f3fa-xysy61', 'f3fa-xyva36', 'f3fa-xyvo792', 'f3fa-xyvu196', 'f3fa-xyxa682', 'f3fa-xyxi861', 'f3fa-xyza82', 'f3fa-xyze42', 'f3fa-xyzo371', 'f3fa-xyzy43', 'f3fa-zabo481', 'f3fa-zace191', 'f3fa-zady11', 'f3fa-zafi63', 'f3fa-zafi99', 'f3fa-zafy01', 'f3fa-zahe49', 'f3fa-zahi037', 'f3fa-zahi82', 'f3fa-zaly82', 'f3fa-zame66', 'f3fa-zamy00', 'f3fa-zany22', 'f3fa-zasy89', 'f3fa-zavo980', 'f3fa-zavu43', 'f3fa-zaxo76', 'f3fa-zebe19', 'f3fa-zebe21', 'f3fa-zefo469', 'f3fa-zego84', 'f3fa-zeha18', 'f3fa-zehy346', 'f3fa-zejo10', 'f3fa-zeke38', 'f3fa-zena88', 'f3fa-zeni13', 'f3fa-zepe04', 'f3fa-zesi57', 'f3fa-zesu28', 'f3fa-zesy46', 'f3fa-zeta584', 'f3fa-zeti66', 'f3fa-zety118', 'f3fa-zety90', 'f3fa-zezu38', 'f3fa-zidu691', 'f3fa-zife206', 'f3fa-zigu963', 'f3fa-zihe762', 'f3fa-zihu30', 'f3fa-zihy25', 'f3fa-ziji68', 'f3fa-ziju36', 'f3fa-zili36', 'f3fa-zima04', 'f3fa-zimo800', 'f3fa-zinu46', 'f3fa-zipi37', 'f3fa-zipi870', 'f3fa-zipy09', 'f3fa-ziqi14', 'f3fa-ziqy19', 'f3fa-zisu949', 'f3fa-zivi22', 'f3fa-zizi69', 'f3fa-zoby58', 'f3fa-zoco97', 'f3fa-zocu61', 'f3fa-zocy92', 'f3fa-zoda11', 'f3fa-zody809', 'f3fa-zofe78', 'f3fa-zofo637', 'f3fa-zoga33', 'f3fa-zogi37', 'f3fa-zogy03', 'f3fa-zohe69', 'f3fa-zoky490', 'f3fa-zolo24', 'f3fa-zoma02', 'f3fa-zomi518', 'f3fa-zomo179', 'f3fa-zomy41', 'f3fa-zona64', 'f3fa-zopa225', 'f3fa-zopu014', 'f3fa-zoqo47', 'f3fa-zoqo956', 'f3fa-zosu</t>
@@ -227,9 +221,6 @@
     <t>{'subrange_est': 3.34, 'subrange_se': 0.03, 'slopes': array([ 88.07, 550.75]), 'intercepts': array([1318.54, -226.71]), 'fitbreaks': array([1.  , 3.34, 9.  ]), 'betas': array([1406.6 ,   88.07,  462.68])}</t>
   </si>
   <si>
-    <t>{'subrange_est': 3.34, 'subrange_se': 0.03, 'slopes': array([ 88.06, 550.75]), 'intercepts': array([1318.54, -226.71]), 'fitbreaks': array([1.  , 3.34, 9.  ]), 'betas': array([1406.6 ,   88.06,  462.68])}</t>
-  </si>
-  <si>
     <t>['sex', 'language']</t>
   </si>
   <si>
@@ -245,17 +236,14 @@
     <t>['IDCode']</t>
   </si>
   <si>
-    <t>[6.2, 31.2, 5.7, 49.0, 6.8, 4.4, 90.5, 5.8, 6.5, 6.0, 6.2, 99.5, 5.8, 6.0, 212.0, 28.2, 5.4, 217.0, 211.0, 5.8]</t>
-  </si>
-  <si>
-    <t>[13.4, 13.2, 15.2, 21.9, 15.6, 16.9, 25.0, 30.0, 18.6, 14.1, 26.9, 14.3, 22.7, 16.0, 14.9, 22.2, 12.0, 19.6, 20.3, 13.3]</t>
+    <t>[4.9, 5.2, 6.9, 3.6, 9.0, 5.1, 3.5, 4.2, 6.9, 5.4, 4.3, 3.5, 3.8, 4.6, 5.9, 4.2, 4.3, 4.0, 3.6, 6.4]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,13 +306,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -362,7 +358,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -396,6 +392,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -430,9 +427,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -605,14 +603,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="P1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:57">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +783,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:57">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -817,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2">
         <v>0.05</v>
@@ -829,79 +827,79 @@
         <v>5</v>
       </c>
       <c r="O2">
-        <v>7</v>
+        <v>609</v>
       </c>
       <c r="P2">
-        <v>7.6</v>
+        <v>750.3</v>
       </c>
       <c r="Q2">
-        <v>20</v>
+        <v>752.9</v>
       </c>
       <c r="R2">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="S2">
-        <v>0.38</v>
+        <v>0.17</v>
       </c>
       <c r="T2">
-        <v>0.55</v>
+        <v>0.22</v>
       </c>
       <c r="U2">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="V2">
-        <v>0.38</v>
+        <v>0.17</v>
       </c>
       <c r="W2">
-        <v>0.55</v>
+        <v>0.22</v>
       </c>
       <c r="X2">
-        <v>1.94</v>
+        <v>2.9</v>
       </c>
       <c r="Y2">
-        <v>2.95</v>
+        <v>3.09</v>
       </c>
       <c r="Z2">
-        <v>2.96</v>
+        <v>3.17</v>
       </c>
       <c r="AA2">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="AB2">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="AC2">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
       <c r="AD2">
-        <v>1.645034224460803</v>
+        <v>0.84340694821128759</v>
       </c>
       <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
         <v>1</v>
       </c>
-      <c r="AF2">
-        <v>2</v>
-      </c>
-      <c r="AG2">
-        <v>2</v>
-      </c>
       <c r="AH2">
-        <v>0.6084158397143784</v>
+        <v>1.472426707994366</v>
       </c>
       <c r="AI2">
-        <v>3.124260826409453</v>
+        <v>1.6832556528053899</v>
       </c>
       <c r="AJ2">
-        <v>0.09543076452835679</v>
+        <v>0.4332438449449974</v>
       </c>
       <c r="AK2">
-        <v>0.1901803652837056</v>
+        <v>0.51426695219207552</v>
       </c>
       <c r="AL2">
-        <v>0.379919773856514</v>
+        <v>0.60964796014111489</v>
       </c>
       <c r="AM2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN2">
         <v>2</v>
@@ -910,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="AP2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ2">
         <v>2</v>
@@ -919,215 +917,42 @@
         <v>2</v>
       </c>
       <c r="AS2">
-        <v>0.3225806451612903</v>
+        <v>0.22580645161290319</v>
       </c>
       <c r="AT2">
-        <v>1.612903225806452</v>
+        <v>1.741935483870968</v>
       </c>
       <c r="AU2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AV2">
-        <v>12.49623840252558</v>
+        <v>6.5402835090955103</v>
       </c>
       <c r="AW2">
         <v>20</v>
       </c>
       <c r="AX2">
-        <v>50.45</v>
+        <v>4.9649999999999999</v>
       </c>
       <c r="AY2">
-        <v>73.59668131104826</v>
+        <v>1.4047330707290979</v>
       </c>
       <c r="AZ2">
-        <v>171.5165407566744</v>
+        <v>7.2757859013493658</v>
       </c>
       <c r="BA2">
-        <v>194.6994953696546</v>
+        <v>7.7182768186290307</v>
       </c>
       <c r="BB2">
-        <v>240.3294377825045</v>
+        <v>8.5892113224810718</v>
       </c>
       <c r="BC2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BD2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BE2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3">
-        <v>0.05</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>5</v>
-      </c>
-      <c r="O3">
-        <v>2212.5</v>
-      </c>
-      <c r="P3">
-        <v>2602.3</v>
-      </c>
-      <c r="Q3">
-        <v>2846.5</v>
-      </c>
-      <c r="R3">
-        <v>0.05</v>
-      </c>
-      <c r="S3">
-        <v>0.05</v>
-      </c>
-      <c r="T3">
-        <v>0.05</v>
-      </c>
-      <c r="U3">
-        <v>0.05</v>
-      </c>
-      <c r="V3">
-        <v>0.05</v>
-      </c>
-      <c r="W3">
-        <v>0.05</v>
-      </c>
-      <c r="X3">
-        <v>2.85</v>
-      </c>
-      <c r="Y3">
-        <v>2.86</v>
-      </c>
-      <c r="Z3">
-        <v>2.89</v>
-      </c>
-      <c r="AA3">
-        <v>0.17</v>
-      </c>
-      <c r="AB3">
-        <v>0.19</v>
-      </c>
-      <c r="AC3">
-        <v>0.2</v>
-      </c>
-      <c r="AD3">
-        <v>0.2493865426837143</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0</v>
-      </c>
-      <c r="AH3">
-        <v>1.780317706315375</v>
-      </c>
-      <c r="AI3">
-        <v>0.9712045483946015</v>
-      </c>
-      <c r="AJ3">
-        <v>0.2862515316151819</v>
-      </c>
-      <c r="AK3">
-        <v>0.3243967337037813</v>
-      </c>
-      <c r="AL3">
-        <v>0.3944759312706554</v>
-      </c>
-      <c r="AM3">
-        <v>2</v>
-      </c>
-      <c r="AN3">
-        <v>3</v>
-      </c>
-      <c r="AO3">
-        <v>3</v>
-      </c>
-      <c r="AP3">
-        <v>2</v>
-      </c>
-      <c r="AQ3">
-        <v>2</v>
-      </c>
-      <c r="AR3">
-        <v>3</v>
-      </c>
-      <c r="AS3">
-        <v>0.4193548387096774</v>
-      </c>
-      <c r="AT3">
-        <v>1.483870967741935</v>
-      </c>
-      <c r="AU3">
-        <v>8</v>
-      </c>
-      <c r="AV3">
-        <v>4.339059189955393</v>
-      </c>
-      <c r="AW3">
-        <v>20</v>
-      </c>
-      <c r="AX3">
-        <v>18.305</v>
-      </c>
-      <c r="AY3">
-        <v>4.965427977526207</v>
-      </c>
-      <c r="AZ3">
-        <v>26.47312902303061</v>
-      </c>
-      <c r="BA3">
-        <v>28.03723883595136</v>
-      </c>
-      <c r="BB3">
-        <v>31.11580418201761</v>
-      </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
-      <c r="BD3">
-        <v>0</v>
-      </c>
-      <c r="BE3">
         <v>0</v>
       </c>
     </row>
@@ -1137,14 +962,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -1224,7 +1051,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1256,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L2">
         <v>0.05</v>
@@ -1265,123 +1092,43 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s">
         <v>61</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>62</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>63</v>
+      </c>
+      <c r="R2" t="s">
         <v>64</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" t="s">
-        <v>68</v>
       </c>
       <c r="S2">
         <v>261303</v>
       </c>
       <c r="T2" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" t="s">
+        <v>66</v>
+      </c>
+      <c r="V2" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" t="s">
         <v>69</v>
       </c>
-      <c r="U2" t="s">
+      <c r="Y2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z2" t="s">
         <v>71</v>
-      </c>
-      <c r="V2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" t="s">
-        <v>73</v>
-      </c>
-      <c r="X2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3">
-        <v>0.05</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P3" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>67</v>
-      </c>
-      <c r="R3" t="s">
-        <v>68</v>
-      </c>
-      <c r="S3">
-        <v>261303</v>
-      </c>
-      <c r="T3" t="s">
-        <v>70</v>
-      </c>
-      <c r="U3" t="s">
-        <v>71</v>
-      </c>
-      <c r="V3" t="s">
-        <v>72</v>
-      </c>
-      <c r="W3" t="s">
-        <v>73</v>
-      </c>
-      <c r="X3" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>